<commit_message>
maj grille de competences
</commit_message>
<xml_diff>
--- a/CVEtDoc/Tableau de synthèse - Epreuve E4 - BTS SIO 2023.xlsx
+++ b/CVEtDoc/Tableau de synthèse - Epreuve E4 - BTS SIO 2023.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ETHAN\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ETHAN\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4900A089-46C4-44ED-AA34-B61EE1E6BDB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E88246CE-D78D-429C-BAAF-65DBABC62DCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,14 +16,14 @@
     <sheet name="Tableau de synthèse Épreuve E4" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Tableau de synthèse Épreuve E4'!$A$1:$H$35</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Tableau de synthèse Épreuve E4'!$A$1:$H$18</definedName>
   </definedNames>
   <calcPr calcId="101716"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="34">
   <si>
     <t>Gérer le patrimoine informatique</t>
   </si>
@@ -86,13 +86,7 @@
 ▸Développer son projet professionnel</t>
   </si>
   <si>
-    <t>Centre de formation :</t>
-  </si>
-  <si>
     <t>▢ SISR</t>
-  </si>
-  <si>
-    <t>▢ SLAM</t>
   </si>
   <si>
     <t xml:space="preserve">Réalisation en cours de formation
@@ -104,12 +98,6 @@
 (intitulé et liste des documents et productions associés)</t>
   </si>
   <si>
-    <t xml:space="preserve">N° candidat : </t>
-  </si>
-  <si>
-    <t xml:space="preserve">NOM et prénom : </t>
-  </si>
-  <si>
     <t>Période (sous la forme du JJ/MM/AA au JJ/MM/AA)</t>
   </si>
   <si>
@@ -119,9 +107,6 @@
     <t>Réalisations en milieu professionnel en cours de seconde année</t>
   </si>
   <si>
-    <t>Adresse URL du portfolio :</t>
-  </si>
-  <si>
     <t>SESSION 2023</t>
   </si>
   <si>
@@ -140,7 +125,25 @@
     <t>Portfolio</t>
   </si>
   <si>
-    <t>Création d'un CV</t>
+    <t>GLPI</t>
+  </si>
+  <si>
+    <t>NOM et prénom : BELLAICHE Ethan</t>
+  </si>
+  <si>
+    <t>Centre de formation : ORT Montreuil</t>
+  </si>
+  <si>
+    <t>Adresse URL du portfolio : https://ethanol55.github.io</t>
+  </si>
+  <si>
+    <t>N° candidat : 02245154174</t>
+  </si>
+  <si>
+    <t>Site Web pour l'entreprise</t>
+  </si>
+  <si>
+    <t>X SLAM</t>
   </si>
 </sst>
 </file>
@@ -213,13 +216,25 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="29">
     <border>
@@ -326,51 +341,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color theme="2" tint="-0.749992370372631"/>
-      </left>
-      <right style="thin">
-        <color theme="2" tint="-0.749992370372631"/>
-      </right>
-      <top style="thin">
-        <color theme="2" tint="-0.749992370372631"/>
-      </top>
-      <bottom style="medium">
-        <color theme="2" tint="-0.749992370372631"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="2" tint="-0.749992370372631"/>
-      </left>
-      <right style="thin">
-        <color theme="2" tint="-0.749992370372631"/>
-      </right>
-      <top style="thin">
-        <color theme="2" tint="-0.749992370372631"/>
-      </top>
-      <bottom style="medium">
-        <color theme="2" tint="-0.749992370372631"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="2" tint="-0.749992370372631"/>
-      </left>
-      <right style="medium">
-        <color theme="2" tint="-0.749992370372631"/>
-      </right>
-      <top style="thin">
-        <color theme="2" tint="-0.749992370372631"/>
-      </top>
-      <bottom style="medium">
-        <color theme="2" tint="-0.749992370372631"/>
-      </bottom>
-      <diagonal/>
-    </border>
     <border diagonalDown="1">
       <left style="medium">
         <color theme="2" tint="-0.749992370372631"/>
@@ -603,6 +573,45 @@
         <color theme="2" tint="-0.749992370372631"/>
       </top>
       <bottom style="medium">
+        <color theme="2" tint="-0.749992370372631"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="2" tint="-0.749992370372631"/>
+      </left>
+      <right style="thin">
+        <color theme="2" tint="-0.749992370372631"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="2" tint="-0.749992370372631"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="2" tint="-0.749992370372631"/>
+      </left>
+      <right style="thin">
+        <color theme="2" tint="-0.749992370372631"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="2" tint="-0.749992370372631"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="2" tint="-0.749992370372631"/>
+      </left>
+      <right style="medium">
+        <color theme="2" tint="-0.749992370372631"/>
+      </right>
+      <top/>
+      <bottom style="thin">
         <color theme="2" tint="-0.749992370372631"/>
       </bottom>
       <diagonal/>
@@ -612,7 +621,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -635,23 +644,11 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -665,22 +662,46 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="17" fontId="8" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -695,28 +716,46 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -724,27 +763,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1088,10 +1106,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AQ81"/>
+  <dimension ref="A1:AQ64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="105" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1104,84 +1122,84 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:43" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24" t="s">
-        <v>26</v>
-      </c>
-      <c r="H1" s="24"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1" s="28"/>
     </row>
     <row r="2" spans="1:43" ht="40.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24"/>
-      <c r="H2" s="24"/>
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="28"/>
     </row>
     <row r="3" spans="1:43" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="36" t="s">
-        <v>21</v>
-      </c>
-      <c r="B3" s="37"/>
-      <c r="C3" s="37"/>
-      <c r="D3" s="37"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="42" t="s">
-        <v>20</v>
-      </c>
-      <c r="G3" s="37"/>
-      <c r="H3" s="43"/>
+      <c r="A3" s="40" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" s="41"/>
+      <c r="C3" s="41"/>
+      <c r="D3" s="41"/>
+      <c r="E3" s="42"/>
+      <c r="F3" s="46" t="s">
+        <v>31</v>
+      </c>
+      <c r="G3" s="41"/>
+      <c r="H3" s="47"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
     </row>
     <row r="4" spans="1:43" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="39" t="s">
+      <c r="A4" s="43" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" s="44"/>
+      <c r="C4" s="44"/>
+      <c r="D4" s="44"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="40"/>
-      <c r="C4" s="40"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="41"/>
-      <c r="F4" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="G4" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="H4" s="21" t="s">
-        <v>17</v>
+      <c r="H4" s="15" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:43" ht="40.049999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="33" t="s">
-        <v>25</v>
-      </c>
-      <c r="B5" s="34"/>
-      <c r="C5" s="34"/>
-      <c r="D5" s="34"/>
-      <c r="E5" s="34"/>
-      <c r="F5" s="34"/>
-      <c r="G5" s="34"/>
-      <c r="H5" s="35"/>
+      <c r="A5" s="37" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" s="38"/>
+      <c r="C5" s="38"/>
+      <c r="D5" s="38"/>
+      <c r="E5" s="38"/>
+      <c r="F5" s="38"/>
+      <c r="G5" s="38"/>
+      <c r="H5" s="39"/>
     </row>
     <row r="6" spans="1:43" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="22" t="s">
-        <v>19</v>
-      </c>
-      <c r="B6" s="31" t="s">
-        <v>22</v>
+      <c r="A6" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="35" t="s">
+        <v>18</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>0</v>
@@ -1203,24 +1221,24 @@
       </c>
     </row>
     <row r="7" spans="1:43" s="2" customFormat="1" ht="325.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="23"/>
-      <c r="B7" s="32"/>
-      <c r="C7" s="44" t="s">
+      <c r="A7" s="27"/>
+      <c r="B7" s="36"/>
+      <c r="C7" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="D7" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="E7" s="8" t="s">
+      <c r="E7" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="F7" s="8" t="s">
+      <c r="F7" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="G7" s="8" t="s">
+      <c r="G7" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="H7" s="9" t="s">
+      <c r="H7" s="25" t="s">
         <v>14</v>
       </c>
       <c r="I7"/>
@@ -1260,16 +1278,16 @@
       <c r="AQ7"/>
     </row>
     <row r="8" spans="1:43" s="2" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A8" s="25" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8" s="26"/>
-      <c r="C8" s="26"/>
-      <c r="D8" s="26"/>
-      <c r="E8" s="26"/>
-      <c r="F8" s="26"/>
-      <c r="G8" s="26"/>
-      <c r="H8" s="27"/>
+      <c r="A8" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="30"/>
+      <c r="C8" s="30"/>
+      <c r="D8" s="30"/>
+      <c r="E8" s="30"/>
+      <c r="F8" s="30"/>
+      <c r="G8" s="30"/>
+      <c r="H8" s="31"/>
       <c r="I8"/>
       <c r="J8"/>
       <c r="K8"/>
@@ -1306,19 +1324,21 @@
       <c r="AP8"/>
       <c r="AQ8"/>
     </row>
-    <row r="9" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="11" t="s">
+    <row r="9" spans="1:43" s="2" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+      <c r="A9" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="B9" s="10"/>
-      <c r="C9" s="16"/>
-      <c r="D9" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="E9" s="17"/>
-      <c r="F9" s="17"/>
-      <c r="G9" s="17"/>
-      <c r="H9" s="18"/>
+      <c r="B9" s="20">
+        <v>44470</v>
+      </c>
+      <c r="C9" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="18"/>
+      <c r="H9" s="19"/>
       <c r="I9"/>
       <c r="J9"/>
       <c r="K9"/>
@@ -1356,22 +1376,16 @@
       <c r="AQ9"/>
     </row>
     <row r="10" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="B10" s="10"/>
-      <c r="C10" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="D10" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="E10" s="17"/>
-      <c r="F10" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="G10" s="17"/>
-      <c r="H10" s="18"/>
+      <c r="A10" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="8"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="22"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="24"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="14"/>
       <c r="I10"/>
       <c r="J10"/>
       <c r="K10"/>
@@ -1409,22 +1423,20 @@
       <c r="AQ10"/>
     </row>
     <row r="11" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="B11" s="10"/>
-      <c r="C11" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="D11" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="E11" s="17"/>
-      <c r="F11" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="G11" s="17"/>
-      <c r="H11" s="18"/>
+      <c r="A11" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="8"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="E11" s="13"/>
+      <c r="F11" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="G11" s="13"/>
+      <c r="H11" s="14"/>
       <c r="I11"/>
       <c r="J11"/>
       <c r="K11"/>
@@ -1462,16 +1474,20 @@
       <c r="AQ11"/>
     </row>
     <row r="12" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="B12" s="10"/>
-      <c r="C12" s="17"/>
-      <c r="D12" s="17"/>
-      <c r="E12" s="17"/>
-      <c r="F12" s="17"/>
-      <c r="G12" s="17"/>
-      <c r="H12" s="18"/>
+      <c r="A12" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" s="8"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="E12" s="13"/>
+      <c r="F12" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="G12" s="13"/>
+      <c r="H12" s="14"/>
       <c r="I12"/>
       <c r="J12"/>
       <c r="K12"/>
@@ -1509,18 +1525,16 @@
       <c r="AQ12"/>
     </row>
     <row r="13" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="B13" s="10"/>
-      <c r="C13" s="17"/>
-      <c r="D13" s="17"/>
-      <c r="E13" s="17"/>
-      <c r="F13" s="17"/>
-      <c r="G13" s="17"/>
-      <c r="H13" s="18" t="s">
-        <v>28</v>
-      </c>
+      <c r="A13" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" s="8"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="22"/>
+      <c r="H13" s="23"/>
       <c r="I13"/>
       <c r="J13"/>
       <c r="K13"/>
@@ -1557,15 +1571,17 @@
       <c r="AP13"/>
       <c r="AQ13"/>
     </row>
-    <row r="14" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="11"/>
-      <c r="B14" s="10"/>
-      <c r="C14" s="17"/>
-      <c r="D14" s="17"/>
-      <c r="E14" s="17"/>
-      <c r="F14" s="17"/>
-      <c r="G14" s="17"/>
-      <c r="H14" s="18"/>
+    <row r="14" spans="1:43" s="2" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+      <c r="A14" s="32" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" s="33"/>
+      <c r="C14" s="33"/>
+      <c r="D14" s="33"/>
+      <c r="E14" s="33"/>
+      <c r="F14" s="33"/>
+      <c r="G14" s="33"/>
+      <c r="H14" s="34"/>
       <c r="I14"/>
       <c r="J14"/>
       <c r="K14"/>
@@ -1603,14 +1619,14 @@
       <c r="AQ14"/>
     </row>
     <row r="15" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="11"/>
-      <c r="B15" s="10"/>
-      <c r="C15" s="17"/>
-      <c r="D15" s="17"/>
-      <c r="E15" s="17"/>
-      <c r="F15" s="17"/>
-      <c r="G15" s="17"/>
-      <c r="H15" s="18"/>
+      <c r="A15" s="9"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
+      <c r="H15" s="14"/>
       <c r="I15"/>
       <c r="J15"/>
       <c r="K15"/>
@@ -1647,15 +1663,17 @@
       <c r="AP15"/>
       <c r="AQ15"/>
     </row>
-    <row r="16" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="11"/>
-      <c r="B16" s="10"/>
-      <c r="C16" s="17"/>
-      <c r="D16" s="17"/>
-      <c r="E16" s="17"/>
-      <c r="F16" s="17"/>
-      <c r="G16" s="17"/>
-      <c r="H16" s="18"/>
+    <row r="16" spans="1:43" s="2" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+      <c r="A16" s="32" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16" s="33"/>
+      <c r="C16" s="33"/>
+      <c r="D16" s="33"/>
+      <c r="E16" s="33"/>
+      <c r="F16" s="33"/>
+      <c r="G16" s="33"/>
+      <c r="H16" s="34"/>
       <c r="I16"/>
       <c r="J16"/>
       <c r="K16"/>
@@ -1693,14 +1711,16 @@
       <c r="AQ16"/>
     </row>
     <row r="17" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="11"/>
-      <c r="B17" s="10"/>
-      <c r="C17" s="17"/>
-      <c r="D17" s="17"/>
-      <c r="E17" s="17"/>
-      <c r="F17" s="17"/>
-      <c r="G17" s="17"/>
-      <c r="H17" s="18"/>
+      <c r="A17" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" s="8"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="22"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
+      <c r="H17" s="14"/>
       <c r="I17"/>
       <c r="J17"/>
       <c r="K17"/>
@@ -1737,15 +1757,15 @@
       <c r="AP17"/>
       <c r="AQ17"/>
     </row>
-    <row r="18" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="11"/>
-      <c r="B18" s="10"/>
-      <c r="C18" s="17"/>
-      <c r="D18" s="17"/>
-      <c r="E18" s="17"/>
-      <c r="F18" s="17"/>
-      <c r="G18" s="17"/>
-      <c r="H18" s="18"/>
+    <row r="18" spans="1:43" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A18" s="5"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
       <c r="I18"/>
       <c r="J18"/>
       <c r="K18"/>
@@ -1782,788 +1802,36 @@
       <c r="AP18"/>
       <c r="AQ18"/>
     </row>
-    <row r="19" spans="1:43" s="2" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A19" s="28" t="s">
-        <v>23</v>
-      </c>
-      <c r="B19" s="29"/>
-      <c r="C19" s="29"/>
-      <c r="D19" s="29"/>
-      <c r="E19" s="29"/>
-      <c r="F19" s="29"/>
-      <c r="G19" s="29"/>
-      <c r="H19" s="30"/>
-      <c r="I19"/>
-      <c r="J19"/>
-      <c r="K19"/>
-      <c r="L19"/>
-      <c r="M19"/>
-      <c r="N19"/>
-      <c r="O19"/>
-      <c r="P19"/>
-      <c r="Q19"/>
-      <c r="R19"/>
-      <c r="S19"/>
-      <c r="T19"/>
-      <c r="U19"/>
-      <c r="V19"/>
-      <c r="W19"/>
-      <c r="X19"/>
-      <c r="Y19"/>
-      <c r="Z19"/>
-      <c r="AA19"/>
-      <c r="AB19"/>
-      <c r="AC19"/>
-      <c r="AD19"/>
-      <c r="AE19"/>
-      <c r="AF19"/>
-      <c r="AG19"/>
-      <c r="AH19"/>
-      <c r="AI19"/>
-      <c r="AJ19"/>
-      <c r="AK19"/>
-      <c r="AL19"/>
-      <c r="AM19"/>
-      <c r="AN19"/>
-      <c r="AO19"/>
-      <c r="AP19"/>
-      <c r="AQ19"/>
-    </row>
-    <row r="20" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="11"/>
-      <c r="B20" s="10"/>
-      <c r="C20" s="17"/>
-      <c r="D20" s="17"/>
-      <c r="E20" s="17"/>
-      <c r="F20" s="17"/>
-      <c r="G20" s="17"/>
-      <c r="H20" s="18"/>
-      <c r="I20"/>
-      <c r="J20"/>
-      <c r="K20"/>
-      <c r="L20"/>
-      <c r="M20"/>
-      <c r="N20"/>
-      <c r="O20"/>
-      <c r="P20"/>
-      <c r="Q20"/>
-      <c r="R20"/>
-      <c r="S20"/>
-      <c r="T20"/>
-      <c r="U20"/>
-      <c r="V20"/>
-      <c r="W20"/>
-      <c r="X20"/>
-      <c r="Y20"/>
-      <c r="Z20"/>
-      <c r="AA20"/>
-      <c r="AB20"/>
-      <c r="AC20"/>
-      <c r="AD20"/>
-      <c r="AE20"/>
-      <c r="AF20"/>
-      <c r="AG20"/>
-      <c r="AH20"/>
-      <c r="AI20"/>
-      <c r="AJ20"/>
-      <c r="AK20"/>
-      <c r="AL20"/>
-      <c r="AM20"/>
-      <c r="AN20"/>
-      <c r="AO20"/>
-      <c r="AP20"/>
-      <c r="AQ20"/>
-    </row>
-    <row r="21" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="11"/>
-      <c r="B21" s="10"/>
-      <c r="C21" s="17"/>
-      <c r="D21" s="17"/>
-      <c r="E21" s="17"/>
-      <c r="F21" s="17"/>
-      <c r="G21" s="17"/>
-      <c r="H21" s="18"/>
-      <c r="I21"/>
-      <c r="J21"/>
-      <c r="K21"/>
-      <c r="L21"/>
-      <c r="M21"/>
-      <c r="N21"/>
-      <c r="O21"/>
-      <c r="P21"/>
-      <c r="Q21"/>
-      <c r="R21"/>
-      <c r="S21"/>
-      <c r="T21"/>
-      <c r="U21"/>
-      <c r="V21"/>
-      <c r="W21"/>
-      <c r="X21"/>
-      <c r="Y21"/>
-      <c r="Z21"/>
-      <c r="AA21"/>
-      <c r="AB21"/>
-      <c r="AC21"/>
-      <c r="AD21"/>
-      <c r="AE21"/>
-      <c r="AF21"/>
-      <c r="AG21"/>
-      <c r="AH21"/>
-      <c r="AI21"/>
-      <c r="AJ21"/>
-      <c r="AK21"/>
-      <c r="AL21"/>
-      <c r="AM21"/>
-      <c r="AN21"/>
-      <c r="AO21"/>
-      <c r="AP21"/>
-      <c r="AQ21"/>
-    </row>
-    <row r="22" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="11"/>
-      <c r="B22" s="10"/>
-      <c r="C22" s="17"/>
-      <c r="D22" s="17"/>
-      <c r="E22" s="17"/>
-      <c r="F22" s="17"/>
-      <c r="G22" s="17"/>
-      <c r="H22" s="18"/>
-      <c r="I22"/>
-      <c r="J22"/>
-      <c r="K22"/>
-      <c r="L22"/>
-      <c r="M22"/>
-      <c r="N22"/>
-      <c r="O22"/>
-      <c r="P22"/>
-      <c r="Q22"/>
-      <c r="R22"/>
-      <c r="S22"/>
-      <c r="T22"/>
-      <c r="U22"/>
-      <c r="V22"/>
-      <c r="W22"/>
-      <c r="X22"/>
-      <c r="Y22"/>
-      <c r="Z22"/>
-      <c r="AA22"/>
-      <c r="AB22"/>
-      <c r="AC22"/>
-      <c r="AD22"/>
-      <c r="AE22"/>
-      <c r="AF22"/>
-      <c r="AG22"/>
-      <c r="AH22"/>
-      <c r="AI22"/>
-      <c r="AJ22"/>
-      <c r="AK22"/>
-      <c r="AL22"/>
-      <c r="AM22"/>
-      <c r="AN22"/>
-      <c r="AO22"/>
-      <c r="AP22"/>
-      <c r="AQ22"/>
-    </row>
-    <row r="23" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="11"/>
-      <c r="B23" s="10"/>
-      <c r="C23" s="17"/>
-      <c r="D23" s="17"/>
-      <c r="E23" s="17"/>
-      <c r="F23" s="17"/>
-      <c r="G23" s="17"/>
-      <c r="H23" s="18"/>
-      <c r="I23"/>
-      <c r="J23"/>
-      <c r="K23"/>
-      <c r="L23"/>
-      <c r="M23"/>
-      <c r="N23"/>
-      <c r="O23"/>
-      <c r="P23"/>
-      <c r="Q23"/>
-      <c r="R23"/>
-      <c r="S23"/>
-      <c r="T23"/>
-      <c r="U23"/>
-      <c r="V23"/>
-      <c r="W23"/>
-      <c r="X23"/>
-      <c r="Y23"/>
-      <c r="Z23"/>
-      <c r="AA23"/>
-      <c r="AB23"/>
-      <c r="AC23"/>
-      <c r="AD23"/>
-      <c r="AE23"/>
-      <c r="AF23"/>
-      <c r="AG23"/>
-      <c r="AH23"/>
-      <c r="AI23"/>
-      <c r="AJ23"/>
-      <c r="AK23"/>
-      <c r="AL23"/>
-      <c r="AM23"/>
-      <c r="AN23"/>
-      <c r="AO23"/>
-      <c r="AP23"/>
-      <c r="AQ23"/>
-    </row>
-    <row r="24" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="11"/>
-      <c r="B24" s="10"/>
-      <c r="C24" s="17"/>
-      <c r="D24" s="17"/>
-      <c r="E24" s="17"/>
-      <c r="F24" s="17"/>
-      <c r="G24" s="17"/>
-      <c r="H24" s="18"/>
-      <c r="I24"/>
-      <c r="J24"/>
-      <c r="K24"/>
-      <c r="L24"/>
-      <c r="M24"/>
-      <c r="N24"/>
-      <c r="O24"/>
-      <c r="P24"/>
-      <c r="Q24"/>
-      <c r="R24"/>
-      <c r="S24"/>
-      <c r="T24"/>
-      <c r="U24"/>
-      <c r="V24"/>
-      <c r="W24"/>
-      <c r="X24"/>
-      <c r="Y24"/>
-      <c r="Z24"/>
-      <c r="AA24"/>
-      <c r="AB24"/>
-      <c r="AC24"/>
-      <c r="AD24"/>
-      <c r="AE24"/>
-      <c r="AF24"/>
-      <c r="AG24"/>
-      <c r="AH24"/>
-      <c r="AI24"/>
-      <c r="AJ24"/>
-      <c r="AK24"/>
-      <c r="AL24"/>
-      <c r="AM24"/>
-      <c r="AN24"/>
-      <c r="AO24"/>
-      <c r="AP24"/>
-      <c r="AQ24"/>
-    </row>
-    <row r="25" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="11"/>
-      <c r="B25" s="10"/>
-      <c r="C25" s="17"/>
-      <c r="D25" s="17"/>
-      <c r="E25" s="17"/>
-      <c r="F25" s="17"/>
-      <c r="G25" s="17"/>
-      <c r="H25" s="18"/>
-      <c r="I25"/>
-      <c r="J25"/>
-      <c r="K25"/>
-      <c r="L25"/>
-      <c r="M25"/>
-      <c r="N25"/>
-      <c r="O25"/>
-      <c r="P25"/>
-      <c r="Q25"/>
-      <c r="R25"/>
-      <c r="S25"/>
-      <c r="T25"/>
-      <c r="U25"/>
-      <c r="V25"/>
-      <c r="W25"/>
-      <c r="X25"/>
-      <c r="Y25"/>
-      <c r="Z25"/>
-      <c r="AA25"/>
-      <c r="AB25"/>
-      <c r="AC25"/>
-      <c r="AD25"/>
-      <c r="AE25"/>
-      <c r="AF25"/>
-      <c r="AG25"/>
-      <c r="AH25"/>
-      <c r="AI25"/>
-      <c r="AJ25"/>
-      <c r="AK25"/>
-      <c r="AL25"/>
-      <c r="AM25"/>
-      <c r="AN25"/>
-      <c r="AO25"/>
-      <c r="AP25"/>
-      <c r="AQ25"/>
-    </row>
-    <row r="26" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="11"/>
-      <c r="B26" s="10"/>
-      <c r="C26" s="17"/>
-      <c r="D26" s="17"/>
-      <c r="E26" s="17"/>
-      <c r="F26" s="17"/>
-      <c r="G26" s="17"/>
-      <c r="H26" s="18"/>
-      <c r="I26"/>
-      <c r="J26"/>
-      <c r="K26"/>
-      <c r="L26"/>
-      <c r="M26"/>
-      <c r="N26"/>
-      <c r="O26"/>
-      <c r="P26"/>
-      <c r="Q26"/>
-      <c r="R26"/>
-      <c r="S26"/>
-      <c r="T26"/>
-      <c r="U26"/>
-      <c r="V26"/>
-      <c r="W26"/>
-      <c r="X26"/>
-      <c r="Y26"/>
-      <c r="Z26"/>
-      <c r="AA26"/>
-      <c r="AB26"/>
-      <c r="AC26"/>
-      <c r="AD26"/>
-      <c r="AE26"/>
-      <c r="AF26"/>
-      <c r="AG26"/>
-      <c r="AH26"/>
-      <c r="AI26"/>
-      <c r="AJ26"/>
-      <c r="AK26"/>
-      <c r="AL26"/>
-      <c r="AM26"/>
-      <c r="AN26"/>
-      <c r="AO26"/>
-      <c r="AP26"/>
-      <c r="AQ26"/>
-    </row>
-    <row r="27" spans="1:43" s="2" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A27" s="28" t="s">
-        <v>24</v>
-      </c>
-      <c r="B27" s="29"/>
-      <c r="C27" s="29"/>
-      <c r="D27" s="29"/>
-      <c r="E27" s="29"/>
-      <c r="F27" s="29"/>
-      <c r="G27" s="29"/>
-      <c r="H27" s="30"/>
-      <c r="I27"/>
-      <c r="J27"/>
-      <c r="K27"/>
-      <c r="L27"/>
-      <c r="M27"/>
-      <c r="N27"/>
-      <c r="O27"/>
-      <c r="P27"/>
-      <c r="Q27"/>
-      <c r="R27"/>
-      <c r="S27"/>
-      <c r="T27"/>
-      <c r="U27"/>
-      <c r="V27"/>
-      <c r="W27"/>
-      <c r="X27"/>
-      <c r="Y27"/>
-      <c r="Z27"/>
-      <c r="AA27"/>
-      <c r="AB27"/>
-      <c r="AC27"/>
-      <c r="AD27"/>
-      <c r="AE27"/>
-      <c r="AF27"/>
-      <c r="AG27"/>
-      <c r="AH27"/>
-      <c r="AI27"/>
-      <c r="AJ27"/>
-      <c r="AK27"/>
-      <c r="AL27"/>
-      <c r="AM27"/>
-      <c r="AN27"/>
-      <c r="AO27"/>
-      <c r="AP27"/>
-      <c r="AQ27"/>
-    </row>
-    <row r="28" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="11"/>
-      <c r="B28" s="10"/>
-      <c r="C28" s="17"/>
-      <c r="D28" s="17"/>
-      <c r="E28" s="17"/>
-      <c r="F28" s="17"/>
-      <c r="G28" s="17"/>
-      <c r="H28" s="18"/>
-      <c r="I28"/>
-      <c r="J28"/>
-      <c r="K28"/>
-      <c r="L28"/>
-      <c r="M28"/>
-      <c r="N28"/>
-      <c r="O28"/>
-      <c r="P28"/>
-      <c r="Q28"/>
-      <c r="R28"/>
-      <c r="S28"/>
-      <c r="T28"/>
-      <c r="U28"/>
-      <c r="V28"/>
-      <c r="W28"/>
-      <c r="X28"/>
-      <c r="Y28"/>
-      <c r="Z28"/>
-      <c r="AA28"/>
-      <c r="AB28"/>
-      <c r="AC28"/>
-      <c r="AD28"/>
-      <c r="AE28"/>
-      <c r="AF28"/>
-      <c r="AG28"/>
-      <c r="AH28"/>
-      <c r="AI28"/>
-      <c r="AJ28"/>
-      <c r="AK28"/>
-      <c r="AL28"/>
-      <c r="AM28"/>
-      <c r="AN28"/>
-      <c r="AO28"/>
-      <c r="AP28"/>
-      <c r="AQ28"/>
-    </row>
-    <row r="29" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="11"/>
-      <c r="B29" s="10"/>
-      <c r="C29" s="17"/>
-      <c r="D29" s="17"/>
-      <c r="E29" s="17"/>
-      <c r="F29" s="17"/>
-      <c r="G29" s="17"/>
-      <c r="H29" s="18"/>
-      <c r="I29"/>
-      <c r="J29"/>
-      <c r="K29"/>
-      <c r="L29"/>
-      <c r="M29"/>
-      <c r="N29"/>
-      <c r="O29"/>
-      <c r="P29"/>
-      <c r="Q29"/>
-      <c r="R29"/>
-      <c r="S29"/>
-      <c r="T29"/>
-      <c r="U29"/>
-      <c r="V29"/>
-      <c r="W29"/>
-      <c r="X29"/>
-      <c r="Y29"/>
-      <c r="Z29"/>
-      <c r="AA29"/>
-      <c r="AB29"/>
-      <c r="AC29"/>
-      <c r="AD29"/>
-      <c r="AE29"/>
-      <c r="AF29"/>
-      <c r="AG29"/>
-      <c r="AH29"/>
-      <c r="AI29"/>
-      <c r="AJ29"/>
-      <c r="AK29"/>
-      <c r="AL29"/>
-      <c r="AM29"/>
-      <c r="AN29"/>
-      <c r="AO29"/>
-      <c r="AP29"/>
-      <c r="AQ29"/>
-    </row>
-    <row r="30" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="11"/>
-      <c r="B30" s="10"/>
-      <c r="C30" s="17"/>
-      <c r="D30" s="17"/>
-      <c r="E30" s="17"/>
-      <c r="F30" s="17"/>
-      <c r="G30" s="17"/>
-      <c r="H30" s="18"/>
-      <c r="I30"/>
-      <c r="J30"/>
-      <c r="K30"/>
-      <c r="L30"/>
-      <c r="M30"/>
-      <c r="N30"/>
-      <c r="O30"/>
-      <c r="P30"/>
-      <c r="Q30"/>
-      <c r="R30"/>
-      <c r="S30"/>
-      <c r="T30"/>
-      <c r="U30"/>
-      <c r="V30"/>
-      <c r="W30"/>
-      <c r="X30"/>
-      <c r="Y30"/>
-      <c r="Z30"/>
-      <c r="AA30"/>
-      <c r="AB30"/>
-      <c r="AC30"/>
-      <c r="AD30"/>
-      <c r="AE30"/>
-      <c r="AF30"/>
-      <c r="AG30"/>
-      <c r="AH30"/>
-      <c r="AI30"/>
-      <c r="AJ30"/>
-      <c r="AK30"/>
-      <c r="AL30"/>
-      <c r="AM30"/>
-      <c r="AN30"/>
-      <c r="AO30"/>
-      <c r="AP30"/>
-      <c r="AQ30"/>
-    </row>
-    <row r="31" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="11"/>
-      <c r="B31" s="10"/>
-      <c r="C31" s="17"/>
-      <c r="D31" s="17"/>
-      <c r="E31" s="17"/>
-      <c r="F31" s="17"/>
-      <c r="G31" s="17"/>
-      <c r="H31" s="18"/>
-      <c r="I31"/>
-      <c r="J31"/>
-      <c r="K31"/>
-      <c r="L31"/>
-      <c r="M31"/>
-      <c r="N31"/>
-      <c r="O31"/>
-      <c r="P31"/>
-      <c r="Q31"/>
-      <c r="R31"/>
-      <c r="S31"/>
-      <c r="T31"/>
-      <c r="U31"/>
-      <c r="V31"/>
-      <c r="W31"/>
-      <c r="X31"/>
-      <c r="Y31"/>
-      <c r="Z31"/>
-      <c r="AA31"/>
-      <c r="AB31"/>
-      <c r="AC31"/>
-      <c r="AD31"/>
-      <c r="AE31"/>
-      <c r="AF31"/>
-      <c r="AG31"/>
-      <c r="AH31"/>
-      <c r="AI31"/>
-      <c r="AJ31"/>
-      <c r="AK31"/>
-      <c r="AL31"/>
-      <c r="AM31"/>
-      <c r="AN31"/>
-      <c r="AO31"/>
-      <c r="AP31"/>
-      <c r="AQ31"/>
-    </row>
-    <row r="32" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="11"/>
-      <c r="B32" s="10"/>
-      <c r="C32" s="17"/>
-      <c r="D32" s="17"/>
-      <c r="E32" s="17"/>
-      <c r="F32" s="17"/>
-      <c r="G32" s="17"/>
-      <c r="H32" s="18"/>
-      <c r="I32"/>
-      <c r="J32"/>
-      <c r="K32"/>
-      <c r="L32"/>
-      <c r="M32"/>
-      <c r="N32"/>
-      <c r="O32"/>
-      <c r="P32"/>
-      <c r="Q32"/>
-      <c r="R32"/>
-      <c r="S32"/>
-      <c r="T32"/>
-      <c r="U32"/>
-      <c r="V32"/>
-      <c r="W32"/>
-      <c r="X32"/>
-      <c r="Y32"/>
-      <c r="Z32"/>
-      <c r="AA32"/>
-      <c r="AB32"/>
-      <c r="AC32"/>
-      <c r="AD32"/>
-      <c r="AE32"/>
-      <c r="AF32"/>
-      <c r="AG32"/>
-      <c r="AH32"/>
-      <c r="AI32"/>
-      <c r="AJ32"/>
-      <c r="AK32"/>
-      <c r="AL32"/>
-      <c r="AM32"/>
-      <c r="AN32"/>
-      <c r="AO32"/>
-      <c r="AP32"/>
-      <c r="AQ32"/>
-    </row>
-    <row r="33" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="11"/>
-      <c r="B33" s="10"/>
-      <c r="C33" s="17"/>
-      <c r="D33" s="17"/>
-      <c r="E33" s="17"/>
-      <c r="F33" s="17"/>
-      <c r="G33" s="17"/>
-      <c r="H33" s="18"/>
-      <c r="I33"/>
-      <c r="J33"/>
-      <c r="K33"/>
-      <c r="L33"/>
-      <c r="M33"/>
-      <c r="N33"/>
-      <c r="O33"/>
-      <c r="P33"/>
-      <c r="Q33"/>
-      <c r="R33"/>
-      <c r="S33"/>
-      <c r="T33"/>
-      <c r="U33"/>
-      <c r="V33"/>
-      <c r="W33"/>
-      <c r="X33"/>
-      <c r="Y33"/>
-      <c r="Z33"/>
-      <c r="AA33"/>
-      <c r="AB33"/>
-      <c r="AC33"/>
-      <c r="AD33"/>
-      <c r="AE33"/>
-      <c r="AF33"/>
-      <c r="AG33"/>
-      <c r="AH33"/>
-      <c r="AI33"/>
-      <c r="AJ33"/>
-      <c r="AK33"/>
-      <c r="AL33"/>
-      <c r="AM33"/>
-      <c r="AN33"/>
-      <c r="AO33"/>
-      <c r="AP33"/>
-      <c r="AQ33"/>
-    </row>
-    <row r="34" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="12"/>
-      <c r="B34" s="13"/>
-      <c r="C34" s="19"/>
-      <c r="D34" s="19"/>
-      <c r="E34" s="19"/>
-      <c r="F34" s="19"/>
-      <c r="G34" s="19"/>
-      <c r="H34" s="20"/>
-      <c r="I34"/>
-      <c r="J34"/>
-      <c r="K34"/>
-      <c r="L34"/>
-      <c r="M34"/>
-      <c r="N34"/>
-      <c r="O34"/>
-      <c r="P34"/>
-      <c r="Q34"/>
-      <c r="R34"/>
-      <c r="S34"/>
-      <c r="T34"/>
-      <c r="U34"/>
-      <c r="V34"/>
-      <c r="W34"/>
-      <c r="X34"/>
-      <c r="Y34"/>
-      <c r="Z34"/>
-      <c r="AA34"/>
-      <c r="AB34"/>
-      <c r="AC34"/>
-      <c r="AD34"/>
-      <c r="AE34"/>
-      <c r="AF34"/>
-      <c r="AG34"/>
-      <c r="AH34"/>
-      <c r="AI34"/>
-      <c r="AJ34"/>
-      <c r="AK34"/>
-      <c r="AL34"/>
-      <c r="AM34"/>
-      <c r="AN34"/>
-      <c r="AO34"/>
-      <c r="AP34"/>
-      <c r="AQ34"/>
-    </row>
-    <row r="35" spans="1:43" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A35" s="5"/>
-      <c r="B35" s="3"/>
-      <c r="C35" s="4"/>
-      <c r="D35" s="4"/>
-      <c r="E35" s="4"/>
-      <c r="F35" s="4"/>
-      <c r="G35" s="4"/>
-      <c r="H35" s="4"/>
-      <c r="I35"/>
-      <c r="J35"/>
-      <c r="K35"/>
-      <c r="L35"/>
-      <c r="M35"/>
-      <c r="N35"/>
-      <c r="O35"/>
-      <c r="P35"/>
-      <c r="Q35"/>
-      <c r="R35"/>
-      <c r="S35"/>
-      <c r="T35"/>
-      <c r="U35"/>
-      <c r="V35"/>
-      <c r="W35"/>
-      <c r="X35"/>
-      <c r="Y35"/>
-      <c r="Z35"/>
-      <c r="AA35"/>
-      <c r="AB35"/>
-      <c r="AC35"/>
-      <c r="AD35"/>
-      <c r="AE35"/>
-      <c r="AF35"/>
-      <c r="AG35"/>
-      <c r="AH35"/>
-      <c r="AI35"/>
-      <c r="AJ35"/>
-      <c r="AK35"/>
-      <c r="AL35"/>
-      <c r="AM35"/>
-      <c r="AN35"/>
-      <c r="AO35"/>
-      <c r="AP35"/>
-      <c r="AQ35"/>
-    </row>
-    <row r="36" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="37" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="38" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="39" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="40" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="41" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="42" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="43" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="44" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="45" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="46" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="47" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="48" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="19" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="21" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="33" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="38" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="39" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="40" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="41" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="42" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="43" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="44" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="45" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="46" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="47" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="48" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="49" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="50" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="51" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -2580,23 +1848,6 @@
     <row r="62" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="63" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="64" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="65" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="66" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="67" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="68" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="69" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="70" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="71" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="72" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="73" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="74" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="75" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="76" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="77" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="78" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="79" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="80" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="81" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="12">
     <mergeCell ref="G1:H1"/>
@@ -2607,8 +1858,8 @@
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="A2:H2"/>
     <mergeCell ref="A8:H8"/>
-    <mergeCell ref="A19:H19"/>
-    <mergeCell ref="A27:H27"/>
+    <mergeCell ref="A14:H14"/>
+    <mergeCell ref="A16:H16"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="A5:H5"/>
   </mergeCells>

</xml_diff>

<commit_message>
maj de la grille de competences
</commit_message>
<xml_diff>
--- a/CVEtDoc/Tableau de synthèse - Epreuve E4 - BTS SIO 2023.xlsx
+++ b/CVEtDoc/Tableau de synthèse - Epreuve E4 - BTS SIO 2023.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ETHAN\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ETHAN\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E88246CE-D78D-429C-BAAF-65DBABC62DCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A3F0DD7-61FD-4744-BAA2-B12BCA7A574A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -153,7 +153,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_-* #,##0.00\ [$€-1]_-;\-* #,##0.00\ [$€-1]_-;_-* &quot;-&quot;??\ [$€-1]_-"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -215,6 +215,11 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -621,7 +626,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -638,12 +643,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -668,9 +667,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -695,8 +691,32 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -704,9 +724,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -740,29 +757,23 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="17" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1108,137 +1119,142 @@
   </sheetPr>
   <dimension ref="A1:AQ64"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="70.44140625" style="1" customWidth="1"/>
     <col min="2" max="2" width="10.77734375" style="1" customWidth="1"/>
-    <col min="3" max="8" width="18.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="37.5546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="25.44140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="27" style="1" customWidth="1"/>
+    <col min="6" max="6" width="25.77734375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="27.6640625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="29.5546875" style="1" customWidth="1"/>
     <col min="9" max="43" width="11.5546875" customWidth="1"/>
     <col min="44" max="16384" width="10.77734375" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:43" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28" t="s">
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="H1" s="28"/>
+      <c r="H1" s="22"/>
     </row>
     <row r="2" spans="1:43" ht="40.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="28" t="s">
+      <c r="A2" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="28"/>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="28"/>
-      <c r="G2" s="28"/>
-      <c r="H2" s="28"/>
+      <c r="B2" s="22"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="22"/>
     </row>
     <row r="3" spans="1:43" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="40" t="s">
+      <c r="A3" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="B3" s="41"/>
-      <c r="C3" s="41"/>
-      <c r="D3" s="41"/>
-      <c r="E3" s="42"/>
-      <c r="F3" s="46" t="s">
+      <c r="B3" s="24"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="G3" s="41"/>
-      <c r="H3" s="47"/>
+      <c r="G3" s="24"/>
+      <c r="H3" s="30"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
     </row>
     <row r="4" spans="1:43" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="43" t="s">
+      <c r="A4" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="B4" s="44"/>
-      <c r="C4" s="44"/>
-      <c r="D4" s="44"/>
-      <c r="E4" s="45"/>
-      <c r="F4" s="10" t="s">
+      <c r="B4" s="27"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="28"/>
+      <c r="F4" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="11" t="s">
+      <c r="G4" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="H4" s="15" t="s">
+      <c r="H4" s="13" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:43" ht="40.049999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="37" t="s">
+      <c r="A5" s="41" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="38"/>
-      <c r="C5" s="38"/>
-      <c r="D5" s="38"/>
-      <c r="E5" s="38"/>
-      <c r="F5" s="38"/>
-      <c r="G5" s="38"/>
-      <c r="H5" s="39"/>
+      <c r="B5" s="42"/>
+      <c r="C5" s="42"/>
+      <c r="D5" s="42"/>
+      <c r="E5" s="42"/>
+      <c r="F5" s="42"/>
+      <c r="G5" s="42"/>
+      <c r="H5" s="43"/>
     </row>
     <row r="6" spans="1:43" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="26" t="s">
+      <c r="A6" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="35" t="s">
+      <c r="B6" s="39" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="47" t="s">
         <v>1</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="E6" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="F6" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="G6" s="6" t="s">
+      <c r="G6" s="47" t="s">
         <v>4</v>
       </c>
-      <c r="H6" s="7" t="s">
+      <c r="H6" s="48" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:43" s="2" customFormat="1" ht="325.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="27"/>
-      <c r="B7" s="36"/>
-      <c r="C7" s="16" t="s">
+    <row r="7" spans="1:43" s="2" customFormat="1" ht="286.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="32"/>
+      <c r="B7" s="40"/>
+      <c r="C7" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="16" t="s">
+      <c r="D7" s="44" t="s">
         <v>10</v>
       </c>
-      <c r="E7" s="16" t="s">
+      <c r="E7" s="44" t="s">
         <v>11</v>
       </c>
-      <c r="F7" s="16" t="s">
+      <c r="F7" s="45" t="s">
         <v>12</v>
       </c>
-      <c r="G7" s="16" t="s">
+      <c r="G7" s="45" t="s">
         <v>13</v>
       </c>
-      <c r="H7" s="25" t="s">
+      <c r="H7" s="46" t="s">
         <v>14</v>
       </c>
       <c r="I7"/>
@@ -1278,16 +1294,16 @@
       <c r="AQ7"/>
     </row>
     <row r="8" spans="1:43" s="2" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A8" s="29" t="s">
+      <c r="A8" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="30"/>
-      <c r="C8" s="30"/>
-      <c r="D8" s="30"/>
-      <c r="E8" s="30"/>
-      <c r="F8" s="30"/>
-      <c r="G8" s="30"/>
-      <c r="H8" s="31"/>
+      <c r="B8" s="34"/>
+      <c r="C8" s="34"/>
+      <c r="D8" s="34"/>
+      <c r="E8" s="34"/>
+      <c r="F8" s="34"/>
+      <c r="G8" s="34"/>
+      <c r="H8" s="35"/>
       <c r="I8"/>
       <c r="J8"/>
       <c r="K8"/>
@@ -1325,20 +1341,20 @@
       <c r="AQ8"/>
     </row>
     <row r="9" spans="1:43" s="2" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A9" s="17" t="s">
+      <c r="A9" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="B9" s="20">
+      <c r="B9" s="17">
         <v>44470</v>
       </c>
-      <c r="C9" s="21" t="s">
+      <c r="C9" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="D9" s="18"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="18"/>
-      <c r="G9" s="18"/>
-      <c r="H9" s="19"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="16"/>
       <c r="I9"/>
       <c r="J9"/>
       <c r="K9"/>
@@ -1376,16 +1392,18 @@
       <c r="AQ9"/>
     </row>
     <row r="10" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="8"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="22"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="24"/>
-      <c r="G10" s="13"/>
-      <c r="H10" s="14"/>
+      <c r="B10" s="49">
+        <v>44562</v>
+      </c>
+      <c r="C10" s="10"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="21"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="12"/>
       <c r="I10"/>
       <c r="J10"/>
       <c r="K10"/>
@@ -1423,20 +1441,22 @@
       <c r="AQ10"/>
     </row>
     <row r="11" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="9" t="s">
+      <c r="A11" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="8"/>
-      <c r="C11" s="13"/>
-      <c r="D11" s="22" t="s">
+      <c r="B11" s="49">
+        <v>44835</v>
+      </c>
+      <c r="C11" s="11"/>
+      <c r="D11" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="E11" s="13"/>
-      <c r="F11" s="22" t="s">
+      <c r="E11" s="11"/>
+      <c r="F11" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="G11" s="13"/>
-      <c r="H11" s="14"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="12"/>
       <c r="I11"/>
       <c r="J11"/>
       <c r="K11"/>
@@ -1474,20 +1494,22 @@
       <c r="AQ11"/>
     </row>
     <row r="12" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="9" t="s">
+      <c r="A12" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B12" s="8"/>
-      <c r="C12" s="13"/>
-      <c r="D12" s="22" t="s">
+      <c r="B12" s="49">
+        <v>44835</v>
+      </c>
+      <c r="C12" s="11"/>
+      <c r="D12" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="E12" s="13"/>
-      <c r="F12" s="22" t="s">
+      <c r="E12" s="11"/>
+      <c r="F12" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="G12" s="13"/>
-      <c r="H12" s="14"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="12"/>
       <c r="I12"/>
       <c r="J12"/>
       <c r="K12"/>
@@ -1525,16 +1547,18 @@
       <c r="AQ12"/>
     </row>
     <row r="13" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="9" t="s">
+      <c r="A13" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="B13" s="8"/>
-      <c r="C13" s="13"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="22"/>
-      <c r="H13" s="23"/>
+      <c r="B13" s="49">
+        <v>44866</v>
+      </c>
+      <c r="C13" s="11"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="19"/>
+      <c r="H13" s="20"/>
       <c r="I13"/>
       <c r="J13"/>
       <c r="K13"/>
@@ -1572,16 +1596,16 @@
       <c r="AQ13"/>
     </row>
     <row r="14" spans="1:43" s="2" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A14" s="32" t="s">
+      <c r="A14" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="B14" s="33"/>
-      <c r="C14" s="33"/>
-      <c r="D14" s="33"/>
-      <c r="E14" s="33"/>
-      <c r="F14" s="33"/>
-      <c r="G14" s="33"/>
-      <c r="H14" s="34"/>
+      <c r="B14" s="37"/>
+      <c r="C14" s="37"/>
+      <c r="D14" s="37"/>
+      <c r="E14" s="37"/>
+      <c r="F14" s="37"/>
+      <c r="G14" s="37"/>
+      <c r="H14" s="38"/>
       <c r="I14"/>
       <c r="J14"/>
       <c r="K14"/>
@@ -1619,14 +1643,14 @@
       <c r="AQ14"/>
     </row>
     <row r="15" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="9"/>
-      <c r="B15" s="8"/>
-      <c r="C15" s="13"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="13"/>
-      <c r="H15" s="14"/>
+      <c r="A15" s="7"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="11"/>
+      <c r="H15" s="12"/>
       <c r="I15"/>
       <c r="J15"/>
       <c r="K15"/>
@@ -1664,16 +1688,16 @@
       <c r="AQ15"/>
     </row>
     <row r="16" spans="1:43" s="2" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A16" s="32" t="s">
+      <c r="A16" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="B16" s="33"/>
-      <c r="C16" s="33"/>
-      <c r="D16" s="33"/>
-      <c r="E16" s="33"/>
-      <c r="F16" s="33"/>
-      <c r="G16" s="33"/>
-      <c r="H16" s="34"/>
+      <c r="B16" s="37"/>
+      <c r="C16" s="37"/>
+      <c r="D16" s="37"/>
+      <c r="E16" s="37"/>
+      <c r="F16" s="37"/>
+      <c r="G16" s="37"/>
+      <c r="H16" s="38"/>
       <c r="I16"/>
       <c r="J16"/>
       <c r="K16"/>
@@ -1711,16 +1735,18 @@
       <c r="AQ16"/>
     </row>
     <row r="17" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="9" t="s">
+      <c r="A17" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B17" s="8"/>
-      <c r="C17" s="13"/>
-      <c r="D17" s="22"/>
-      <c r="E17" s="13"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="13"/>
-      <c r="H17" s="14"/>
+      <c r="B17" s="49">
+        <v>44927</v>
+      </c>
+      <c r="C17" s="11"/>
+      <c r="D17" s="19"/>
+      <c r="E17" s="11"/>
+      <c r="F17" s="11"/>
+      <c r="G17" s="11"/>
+      <c r="H17" s="12"/>
       <c r="I17"/>
       <c r="J17"/>
       <c r="K17"/>
@@ -1850,11 +1876,6 @@
     <row r="64" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A3:E3"/>
-    <mergeCell ref="A4:E4"/>
-    <mergeCell ref="F3:H3"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="A2:H2"/>
     <mergeCell ref="A8:H8"/>
@@ -1862,11 +1883,16 @@
     <mergeCell ref="A16:H16"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="A5:H5"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A3:E3"/>
+    <mergeCell ref="A4:E4"/>
+    <mergeCell ref="F3:H3"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.19685039370078741" right="0.19685039370078741" top="0.19685039370078741" bottom="0.19685039370078741" header="0.51181102362204722" footer="0.51181102362204722"/>
-  <pageSetup paperSize="9" scale="48" orientation="portrait"/>
+  <pageSetup paperSize="9" scale="57" orientation="landscape" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
</xml_diff>